<commit_message>
Refactor to include school/centre field. Made improvements on UI like the add course button logic and also removed the underline of the text of the download and logout button
</commit_message>
<xml_diff>
--- a/app/files/Part-Time Lecturer Requisition Form - template.xlsx
+++ b/app/files/Part-Time Lecturer Requisition Form - template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Capstone Project\coursepdfextractor\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Capstone Project\app\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D850513-61CA-4FFD-800D-44C4F7E1E290}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EE67AA5-3B78-4EA8-A11D-798FFD9541CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,15 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="37">
   <si>
     <t>Part-Time Lecturer Requisition Form</t>
   </si>
   <si>
     <t xml:space="preserve">School/ Centre: </t>
-  </si>
-  <si>
-    <t>SOC</t>
   </si>
   <si>
     <t xml:space="preserve">Subject Title: </t>
@@ -286,7 +283,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -321,43 +318,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial Narrow"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Arial Narrow"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="MS Sans Serif"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial Narrow"/>
-      <family val="2"/>
-    </font>
-    <font>
       <i/>
       <sz val="12"/>
       <color theme="1"/>
@@ -365,23 +325,11 @@
       <family val="2"/>
     </font>
     <font>
+      <u/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Blackadder ITC"/>
-      <family val="5"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Algerian"/>
-      <family val="5"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Book Antiqua"/>
-      <family val="1"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -561,7 +509,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -580,44 +528,25 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -631,21 +560,29 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -974,7 +911,7 @@
   <dimension ref="A3:L77"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="45" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
@@ -990,20 +927,20 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:12">
-      <c r="A3" s="39" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
-      <c r="L3" s="39"/>
+      <c r="A3" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="2"/>
@@ -1024,9 +961,7 @@
       <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>2</v>
-      </c>
+      <c r="C5" s="4"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -1039,16 +974,16 @@
     </row>
     <row r="6" spans="1:12" ht="32.1" customHeight="1">
       <c r="B6" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" s="5"/>
-      <c r="G6" s="17" t="s">
-        <v>32</v>
+      <c r="G6" s="15" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="21.95" customHeight="1">
       <c r="B7" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="9.9499999999999993" customHeight="1">
@@ -1063,174 +998,174 @@
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
-      <c r="L9" s="22"/>
+      <c r="L9" s="17"/>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="8"/>
       <c r="B10" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="10"/>
+        <v>2</v>
+      </c>
+      <c r="C10" s="34"/>
       <c r="H10" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="I10" s="23"/>
-      <c r="L10" s="24"/>
+        <v>15</v>
+      </c>
+      <c r="I10" s="34"/>
+      <c r="L10" s="18"/>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="8"/>
       <c r="B11" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="11"/>
-      <c r="L11" s="24"/>
+        <v>30</v>
+      </c>
+      <c r="D11" s="35"/>
+      <c r="L11" s="18"/>
     </row>
     <row r="12" spans="1:12" ht="9.9499999999999993" customHeight="1">
       <c r="A12" s="8"/>
-      <c r="L12" s="24"/>
+      <c r="L12" s="18"/>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="8"/>
       <c r="B13" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="L13" s="24"/>
+        <v>33</v>
+      </c>
+      <c r="L13" s="18"/>
     </row>
     <row r="14" spans="1:12" ht="9.9499999999999993" customHeight="1">
       <c r="A14" s="8"/>
-      <c r="L14" s="24"/>
+      <c r="L14" s="18"/>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="8"/>
       <c r="B15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="10"/>
+      <c r="E15" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D15" s="12"/>
-      <c r="E15" s="1" t="s">
+      <c r="G15" s="10"/>
+      <c r="H15" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G15" s="12"/>
-      <c r="H15" s="1" t="s">
+      <c r="I15" s="10">
+        <f>D15*G15</f>
+        <v>0</v>
+      </c>
+      <c r="J15" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="I15" s="12">
-        <f>D15*G15</f>
-        <v>0</v>
-      </c>
-      <c r="J15" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="L15" s="24"/>
+      <c r="L15" s="18"/>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="8"/>
       <c r="B16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" s="12"/>
+        <v>7</v>
+      </c>
+      <c r="D16" s="10"/>
       <c r="E16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G16" s="10"/>
+      <c r="H16" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G16" s="12"/>
-      <c r="H16" s="1" t="s">
+      <c r="I16" s="10">
+        <f t="shared" ref="I16:I18" si="0">D16*G16</f>
+        <v>0</v>
+      </c>
+      <c r="J16" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="I16" s="12">
-        <f t="shared" ref="I16:I18" si="0">D16*G16</f>
-        <v>0</v>
-      </c>
-      <c r="J16" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="L16" s="24"/>
+      <c r="L16" s="18"/>
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="8"/>
       <c r="B17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="12"/>
+        <v>8</v>
+      </c>
+      <c r="D17" s="10"/>
       <c r="E17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17" s="10"/>
+      <c r="H17" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G17" s="12"/>
-      <c r="H17" s="1" t="s">
+      <c r="I17" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J17" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="I17" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J17" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="L17" s="24"/>
+      <c r="L17" s="18"/>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="8"/>
       <c r="B18" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="12"/>
+        <v>9</v>
+      </c>
+      <c r="D18" s="10"/>
       <c r="E18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G18" s="10"/>
+      <c r="H18" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G18" s="12"/>
-      <c r="H18" s="1" t="s">
+      <c r="I18" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J18" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="I18" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J18" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="L18" s="24"/>
+      <c r="L18" s="18"/>
     </row>
     <row r="19" spans="1:12" ht="9.9499999999999993" customHeight="1">
       <c r="A19" s="8"/>
-      <c r="L19" s="24"/>
+      <c r="L19" s="18"/>
     </row>
     <row r="20" spans="1:12">
       <c r="A20" s="8"/>
-      <c r="B20" s="35" t="s">
+      <c r="B20" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="25"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="36"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="14" t="s">
+      <c r="F20" s="12"/>
+      <c r="G20" s="11">
+        <f>SUM(I15:I19)</f>
+        <v>0</v>
+      </c>
+      <c r="H20" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="F20" s="14"/>
-      <c r="G20" s="13">
-        <f>SUM(I15:I19)</f>
-        <v>0</v>
-      </c>
-      <c r="H20" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I20" s="14"/>
-      <c r="J20" s="37">
+      <c r="I20" s="12"/>
+      <c r="J20" s="26">
         <f>D20*G20</f>
         <v>0</v>
       </c>
-      <c r="K20" s="38"/>
-      <c r="L20" s="24"/>
+      <c r="K20" s="27"/>
+      <c r="L20" s="18"/>
     </row>
     <row r="21" spans="1:12" ht="9.9499999999999993" customHeight="1">
-      <c r="A21" s="15"/>
-      <c r="B21" s="16"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="16"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="16"/>
-      <c r="K21" s="16"/>
-      <c r="L21" s="26"/>
+      <c r="A21" s="13"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="20"/>
     </row>
     <row r="23" spans="1:12" ht="9.9499999999999993" customHeight="1">
       <c r="A23" s="6"/>
@@ -1244,175 +1179,175 @@
       <c r="I23" s="7"/>
       <c r="J23" s="7"/>
       <c r="K23" s="7"/>
-      <c r="L23" s="22"/>
+      <c r="L23" s="17"/>
     </row>
     <row r="24" spans="1:12">
       <c r="A24" s="8"/>
-      <c r="B24" s="17" t="s">
+      <c r="B24" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="36"/>
+      <c r="D24" s="37"/>
+      <c r="H24" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="41"/>
-      <c r="D24" s="42"/>
-      <c r="H24" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I24" s="27"/>
-      <c r="L24" s="24"/>
-    </row>
-    <row r="25" spans="1:12" ht="18">
+      <c r="I24" s="38"/>
+      <c r="L24" s="18"/>
+    </row>
+    <row r="25" spans="1:12">
       <c r="A25" s="8"/>
       <c r="B25" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D25" s="18"/>
-      <c r="L25" s="24"/>
+        <v>34</v>
+      </c>
+      <c r="D25" s="16"/>
+      <c r="L25" s="18"/>
     </row>
     <row r="26" spans="1:12" ht="9.9499999999999993" customHeight="1">
       <c r="A26" s="8"/>
-      <c r="L26" s="24"/>
+      <c r="L26" s="18"/>
     </row>
     <row r="27" spans="1:12">
       <c r="A27" s="8"/>
       <c r="B27" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="L27" s="24"/>
+        <v>35</v>
+      </c>
+      <c r="L27" s="18"/>
     </row>
     <row r="28" spans="1:12" ht="9.9499999999999993" customHeight="1">
       <c r="A28" s="8"/>
-      <c r="L28" s="24"/>
+      <c r="L28" s="18"/>
     </row>
     <row r="29" spans="1:12">
       <c r="A29" s="8"/>
       <c r="B29" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D29" s="10"/>
+      <c r="E29" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D29" s="12"/>
-      <c r="E29" s="1" t="s">
+      <c r="G29" s="10"/>
+      <c r="H29" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G29" s="12"/>
-      <c r="H29" s="1" t="s">
+      <c r="I29" s="10">
+        <f>D29*G29</f>
+        <v>0</v>
+      </c>
+      <c r="J29" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="I29" s="12">
-        <f>D29*G29</f>
-        <v>0</v>
-      </c>
-      <c r="J29" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="L29" s="24"/>
+      <c r="L29" s="18"/>
     </row>
     <row r="30" spans="1:12">
       <c r="A30" s="8"/>
       <c r="B30" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D30" s="12"/>
+        <v>7</v>
+      </c>
+      <c r="D30" s="10"/>
       <c r="E30" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G30" s="10"/>
+      <c r="H30" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G30" s="12"/>
-      <c r="H30" s="1" t="s">
+      <c r="I30" s="10">
+        <f t="shared" ref="I30:I32" si="1">D30*G30</f>
+        <v>0</v>
+      </c>
+      <c r="J30" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="I30" s="12">
-        <f t="shared" ref="I30:I32" si="1">D30*G30</f>
-        <v>0</v>
-      </c>
-      <c r="J30" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="L30" s="24"/>
+      <c r="L30" s="18"/>
     </row>
     <row r="31" spans="1:12">
       <c r="A31" s="8"/>
       <c r="B31" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D31" s="12"/>
+        <v>8</v>
+      </c>
+      <c r="D31" s="10"/>
       <c r="E31" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G31" s="10"/>
+      <c r="H31" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G31" s="12"/>
-      <c r="H31" s="1" t="s">
+      <c r="I31" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J31" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="I31" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J31" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="L31" s="24"/>
+      <c r="L31" s="18"/>
     </row>
     <row r="32" spans="1:12">
       <c r="A32" s="8"/>
       <c r="B32" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D32" s="12"/>
+        <v>9</v>
+      </c>
+      <c r="D32" s="10"/>
       <c r="E32" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G32" s="10"/>
+      <c r="H32" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G32" s="12"/>
-      <c r="H32" s="1" t="s">
+      <c r="I32" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J32" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="I32" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J32" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="L32" s="24"/>
+      <c r="L32" s="18"/>
     </row>
     <row r="33" spans="1:12" ht="9.9499999999999993" customHeight="1">
       <c r="A33" s="8"/>
-      <c r="L33" s="24"/>
+      <c r="L33" s="18"/>
     </row>
     <row r="34" spans="1:12">
       <c r="A34" s="8"/>
-      <c r="B34" s="35" t="s">
+      <c r="B34" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" s="25"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C34" s="36"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="14" t="s">
+      <c r="F34" s="12"/>
+      <c r="G34" s="11">
+        <f>SUM(I29:I33)</f>
+        <v>0</v>
+      </c>
+      <c r="H34" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="F34" s="14"/>
-      <c r="G34" s="13">
-        <f>SUM(I29:I33)</f>
-        <v>0</v>
-      </c>
-      <c r="H34" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I34" s="14"/>
-      <c r="J34" s="37">
+      <c r="I34" s="12"/>
+      <c r="J34" s="26">
         <f>D34*G34</f>
         <v>0</v>
       </c>
-      <c r="K34" s="38"/>
-      <c r="L34" s="24"/>
+      <c r="K34" s="27"/>
+      <c r="L34" s="18"/>
     </row>
     <row r="35" spans="1:12" ht="9.9499999999999993" customHeight="1">
-      <c r="A35" s="15"/>
-      <c r="B35" s="16"/>
-      <c r="C35" s="16"/>
-      <c r="D35" s="16"/>
-      <c r="E35" s="16"/>
-      <c r="F35" s="16"/>
-      <c r="G35" s="16"/>
-      <c r="H35" s="16"/>
-      <c r="I35" s="16"/>
-      <c r="J35" s="16"/>
-      <c r="K35" s="16"/>
-      <c r="L35" s="26"/>
+      <c r="A35" s="13"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="14"/>
+      <c r="I35" s="14"/>
+      <c r="J35" s="14"/>
+      <c r="K35" s="14"/>
+      <c r="L35" s="20"/>
     </row>
     <row r="37" spans="1:12" ht="9.9499999999999993" customHeight="1">
       <c r="A37" s="6"/>
@@ -1426,201 +1361,201 @@
       <c r="I37" s="7"/>
       <c r="J37" s="7"/>
       <c r="K37" s="7"/>
-      <c r="L37" s="22"/>
+      <c r="L37" s="17"/>
     </row>
     <row r="38" spans="1:12">
       <c r="A38" s="8"/>
-      <c r="B38" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C38" s="30"/>
-      <c r="H38" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="I38" s="27"/>
-      <c r="L38" s="24"/>
+      <c r="B38" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C38" s="22"/>
+      <c r="H38" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="I38" s="38"/>
+      <c r="L38" s="18"/>
     </row>
     <row r="39" spans="1:12">
       <c r="A39" s="8"/>
-      <c r="B39" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="D39" s="19"/>
-      <c r="L39" s="24"/>
+      <c r="B39" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D39" s="16"/>
+      <c r="L39" s="18"/>
     </row>
     <row r="40" spans="1:12" ht="9.9499999999999993" customHeight="1">
       <c r="A40" s="8"/>
-      <c r="L40" s="24"/>
+      <c r="L40" s="18"/>
     </row>
     <row r="41" spans="1:12">
       <c r="A41" s="8"/>
-      <c r="B41" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="L41" s="24"/>
+      <c r="B41" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="L41" s="18"/>
     </row>
     <row r="42" spans="1:12" ht="9.9499999999999993" customHeight="1">
       <c r="A42" s="8"/>
-      <c r="L42" s="24"/>
+      <c r="L42" s="18"/>
     </row>
     <row r="43" spans="1:12">
       <c r="A43" s="8"/>
       <c r="B43" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D43" s="10"/>
+      <c r="E43" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D43" s="12"/>
-      <c r="E43" s="1" t="s">
+      <c r="G43" s="10"/>
+      <c r="H43" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G43" s="12"/>
-      <c r="H43" s="1" t="s">
+      <c r="I43" s="10">
+        <f>D43*G43</f>
+        <v>0</v>
+      </c>
+      <c r="J43" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="I43" s="12">
-        <f>D43*G43</f>
-        <v>0</v>
-      </c>
-      <c r="J43" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="L43" s="24"/>
+      <c r="L43" s="18"/>
     </row>
     <row r="44" spans="1:12">
       <c r="A44" s="8"/>
       <c r="B44" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D44" s="12"/>
+        <v>7</v>
+      </c>
+      <c r="D44" s="10"/>
       <c r="E44" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G44" s="10"/>
+      <c r="H44" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G44" s="12"/>
-      <c r="H44" s="1" t="s">
+      <c r="I44" s="10">
+        <f t="shared" ref="I44:I46" si="2">D44*G44</f>
+        <v>0</v>
+      </c>
+      <c r="J44" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="I44" s="12">
-        <f t="shared" ref="I44:I46" si="2">D44*G44</f>
-        <v>0</v>
-      </c>
-      <c r="J44" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="L44" s="24"/>
+      <c r="L44" s="18"/>
     </row>
     <row r="45" spans="1:12">
       <c r="A45" s="8"/>
       <c r="B45" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D45" s="12"/>
+        <v>8</v>
+      </c>
+      <c r="D45" s="10"/>
       <c r="E45" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G45" s="10"/>
+      <c r="H45" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G45" s="12"/>
-      <c r="H45" s="1" t="s">
+      <c r="I45" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J45" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="I45" s="12">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J45" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="L45" s="24"/>
+      <c r="L45" s="18"/>
     </row>
     <row r="46" spans="1:12">
       <c r="A46" s="8"/>
       <c r="B46" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D46" s="12"/>
+        <v>9</v>
+      </c>
+      <c r="D46" s="10"/>
       <c r="E46" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G46" s="10"/>
+      <c r="H46" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G46" s="12"/>
-      <c r="H46" s="1" t="s">
+      <c r="I46" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J46" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="I46" s="12">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J46" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="L46" s="24"/>
+      <c r="L46" s="18"/>
     </row>
     <row r="47" spans="1:12" ht="9.9499999999999993" customHeight="1">
       <c r="A47" s="8"/>
-      <c r="L47" s="24"/>
+      <c r="L47" s="18"/>
     </row>
     <row r="48" spans="1:12">
       <c r="A48" s="8"/>
-      <c r="B48" s="35" t="s">
+      <c r="B48" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C48" s="25"/>
+      <c r="D48" s="11"/>
+      <c r="E48" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C48" s="36"/>
-      <c r="D48" s="13"/>
-      <c r="E48" s="14" t="s">
+      <c r="F48" s="12"/>
+      <c r="G48" s="11">
+        <f>SUM(I43:I47)</f>
+        <v>0</v>
+      </c>
+      <c r="H48" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="F48" s="14"/>
-      <c r="G48" s="13">
-        <f>SUM(I43:I47)</f>
-        <v>0</v>
-      </c>
-      <c r="H48" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I48" s="14"/>
-      <c r="J48" s="37">
+      <c r="I48" s="12"/>
+      <c r="J48" s="26">
         <f>D48*G48</f>
         <v>0</v>
       </c>
-      <c r="K48" s="38"/>
-      <c r="L48" s="24"/>
+      <c r="K48" s="27"/>
+      <c r="L48" s="18"/>
     </row>
     <row r="49" spans="1:12" ht="9.9499999999999993" customHeight="1">
-      <c r="A49" s="15"/>
-      <c r="B49" s="16"/>
-      <c r="C49" s="16"/>
-      <c r="D49" s="16"/>
-      <c r="E49" s="16"/>
-      <c r="F49" s="16"/>
-      <c r="G49" s="16"/>
-      <c r="H49" s="16"/>
-      <c r="I49" s="16"/>
-      <c r="J49" s="16"/>
-      <c r="K49" s="16"/>
-      <c r="L49" s="26"/>
+      <c r="A49" s="13"/>
+      <c r="B49" s="14"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
+      <c r="H49" s="14"/>
+      <c r="I49" s="14"/>
+      <c r="J49" s="14"/>
+      <c r="K49" s="14"/>
+      <c r="L49" s="20"/>
     </row>
     <row r="50" spans="1:12" ht="9.9499999999999993" customHeight="1"/>
     <row r="51" spans="1:12">
       <c r="A51" s="8"/>
-      <c r="B51" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="C51" s="20"/>
-      <c r="H51" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="I51" s="27"/>
+      <c r="B51" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C51" s="34"/>
+      <c r="H51" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="I51" s="38"/>
     </row>
     <row r="52" spans="1:12" ht="16.5" customHeight="1">
       <c r="A52" s="8"/>
-      <c r="B52" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="D52" s="21"/>
+      <c r="B52" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D52" s="16"/>
     </row>
     <row r="53" spans="1:12" ht="16.5" customHeight="1">
       <c r="A53" s="8"/>
     </row>
     <row r="54" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="A54" s="8"/>
-      <c r="B54" s="17" t="s">
-        <v>36</v>
+      <c r="B54" s="15" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="55" spans="1:12" ht="14.45" customHeight="1">
@@ -1629,85 +1564,85 @@
     <row r="56" spans="1:12">
       <c r="A56" s="8"/>
       <c r="B56" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D56" s="10"/>
+      <c r="E56" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D56" s="12"/>
-      <c r="E56" s="1" t="s">
+      <c r="G56" s="10"/>
+      <c r="H56" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G56" s="12"/>
-      <c r="H56" s="1" t="s">
+      <c r="I56" s="10">
+        <f>D56*G56</f>
+        <v>0</v>
+      </c>
+      <c r="J56" s="19" t="s">
         <v>6</v>
-      </c>
-      <c r="I56" s="12">
-        <f>D56*G56</f>
-        <v>0</v>
-      </c>
-      <c r="J56" s="25" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="57" spans="1:12">
       <c r="A57" s="8"/>
       <c r="B57" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D57" s="12"/>
+        <v>7</v>
+      </c>
+      <c r="D57" s="10"/>
       <c r="E57" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G57" s="10"/>
+      <c r="H57" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G57" s="12"/>
-      <c r="H57" s="1" t="s">
+      <c r="I57" s="10">
+        <f t="shared" ref="I57:I59" si="3">D57*G57</f>
+        <v>0</v>
+      </c>
+      <c r="J57" s="19" t="s">
         <v>6</v>
-      </c>
-      <c r="I57" s="12">
-        <f t="shared" ref="I57:I59" si="3">D57*G57</f>
-        <v>0</v>
-      </c>
-      <c r="J57" s="25" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="58" spans="1:12">
       <c r="A58" s="8"/>
       <c r="B58" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D58" s="12"/>
+        <v>8</v>
+      </c>
+      <c r="D58" s="10"/>
       <c r="E58" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G58" s="10"/>
+      <c r="H58" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G58" s="12"/>
-      <c r="H58" s="1" t="s">
+      <c r="I58" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J58" s="19" t="s">
         <v>6</v>
-      </c>
-      <c r="I58" s="12">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J58" s="25" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="59" spans="1:12">
       <c r="A59" s="8"/>
       <c r="B59" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D59" s="12"/>
+        <v>9</v>
+      </c>
+      <c r="D59" s="10"/>
       <c r="E59" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G59" s="10"/>
+      <c r="H59" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G59" s="12"/>
-      <c r="H59" s="1" t="s">
+      <c r="I59" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J59" s="19" t="s">
         <v>6</v>
-      </c>
-      <c r="I59" s="12">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J59" s="25" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="60" spans="1:12">
@@ -1715,181 +1650,168 @@
     </row>
     <row r="61" spans="1:12">
       <c r="A61" s="8"/>
-      <c r="B61" s="35" t="s">
+      <c r="B61" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C61" s="25"/>
+      <c r="D61" s="11"/>
+      <c r="E61" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C61" s="36"/>
-      <c r="D61" s="13"/>
-      <c r="E61" s="14" t="s">
+      <c r="F61" s="12"/>
+      <c r="G61" s="11">
+        <f>SUM(I56:I60)</f>
+        <v>0</v>
+      </c>
+      <c r="H61" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="F61" s="14"/>
-      <c r="G61" s="13">
-        <f>SUM(I56:I60)</f>
-        <v>0</v>
-      </c>
-      <c r="H61" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I61" s="14"/>
-      <c r="J61" s="37">
+      <c r="I61" s="12"/>
+      <c r="J61" s="26">
         <f>D61*G61</f>
         <v>0</v>
       </c>
-      <c r="K61" s="38"/>
+      <c r="K61" s="27"/>
     </row>
     <row r="62" spans="1:12">
-      <c r="A62" s="15"/>
-      <c r="B62" s="16"/>
-      <c r="C62" s="16"/>
-      <c r="D62" s="16"/>
-      <c r="E62" s="16"/>
-      <c r="F62" s="16"/>
-      <c r="G62" s="16"/>
-      <c r="H62" s="16"/>
-      <c r="I62" s="16"/>
-      <c r="J62" s="16"/>
-      <c r="K62" s="16"/>
-    </row>
-    <row r="63" spans="1:12">
-      <c r="A63" s="40"/>
-      <c r="B63" s="40"/>
-      <c r="C63" s="40"/>
-      <c r="D63" s="40"/>
-      <c r="E63" s="40"/>
-      <c r="F63" s="40"/>
-      <c r="G63" s="40"/>
-      <c r="H63" s="40"/>
-      <c r="I63" s="40"/>
-      <c r="J63" s="40"/>
-      <c r="K63" s="40"/>
+      <c r="A62" s="13"/>
+      <c r="B62" s="14"/>
+      <c r="C62" s="14"/>
+      <c r="D62" s="14"/>
+      <c r="E62" s="14"/>
+      <c r="F62" s="14"/>
+      <c r="G62" s="14"/>
+      <c r="H62" s="14"/>
+      <c r="I62" s="14"/>
+      <c r="J62" s="14"/>
+      <c r="K62" s="14"/>
     </row>
     <row r="65" spans="2:11">
-      <c r="G65" s="43" t="s">
-        <v>37</v>
-      </c>
-      <c r="H65" s="44"/>
-      <c r="I65" s="45">
+      <c r="G65" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="H65" s="32"/>
+      <c r="I65" s="28">
         <f>SUM(J20,J34,J48,J61)</f>
         <v>0</v>
       </c>
-      <c r="J65" s="45"/>
+      <c r="J65" s="28"/>
     </row>
     <row r="66" spans="2:11">
-      <c r="I66" s="28"/>
-      <c r="J66" s="28"/>
+      <c r="I66" s="21"/>
+      <c r="J66" s="21"/>
     </row>
     <row r="67" spans="2:11" ht="15.95" customHeight="1"/>
     <row r="68" spans="2:11">
       <c r="B68" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E68" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E68" s="1" t="s">
+      <c r="I68" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I68" s="1" t="s">
+    </row>
+    <row r="69" spans="2:11">
+      <c r="I69" s="2"/>
+    </row>
+    <row r="70" spans="2:11">
+      <c r="B70" s="33"/>
+      <c r="C70" s="33"/>
+      <c r="E70" s="33"/>
+      <c r="F70" s="33"/>
+      <c r="I70" s="1" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="69" spans="2:11" ht="17.25">
-      <c r="I69" s="29"/>
-    </row>
-    <row r="70" spans="2:11" ht="17.25">
-      <c r="B70" s="31"/>
-      <c r="C70" s="31"/>
-      <c r="E70" s="32"/>
-      <c r="F70" s="32"/>
-      <c r="I70" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="71" spans="2:11">
       <c r="B71" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E71" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E71" s="1" t="s">
+      <c r="I71" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="I71" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="72" spans="2:11">
       <c r="B72" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E72" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E72" s="1" t="s">
+      <c r="I72" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="I72" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="74" spans="2:11" ht="15.6" customHeight="1">
       <c r="B74" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="75" spans="2:11" ht="15.6" customHeight="1">
+      <c r="B75" s="30" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="75" spans="2:11" ht="15.6" customHeight="1">
-      <c r="B75" s="33" t="s">
+      <c r="C75" s="30"/>
+      <c r="D75" s="30"/>
+      <c r="E75" s="30"/>
+      <c r="F75" s="30"/>
+      <c r="G75" s="30"/>
+      <c r="H75" s="30"/>
+      <c r="I75" s="30"/>
+      <c r="J75" s="30"/>
+      <c r="K75" s="30"/>
+    </row>
+    <row r="76" spans="2:11">
+      <c r="B76" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="C75" s="33"/>
-      <c r="D75" s="33"/>
-      <c r="E75" s="33"/>
-      <c r="F75" s="33"/>
-      <c r="G75" s="33"/>
-      <c r="H75" s="33"/>
-      <c r="I75" s="33"/>
-      <c r="J75" s="33"/>
-      <c r="K75" s="33"/>
-    </row>
-    <row r="76" spans="2:11">
-      <c r="B76" s="33" t="s">
+      <c r="C76" s="30"/>
+      <c r="D76" s="30"/>
+      <c r="E76" s="30"/>
+      <c r="F76" s="30"/>
+      <c r="G76" s="30"/>
+      <c r="H76" s="30"/>
+      <c r="I76" s="30"/>
+      <c r="J76" s="30"/>
+      <c r="K76" s="30"/>
+    </row>
+    <row r="77" spans="2:11">
+      <c r="B77" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="C76" s="33"/>
-      <c r="D76" s="33"/>
-      <c r="E76" s="33"/>
-      <c r="F76" s="33"/>
-      <c r="G76" s="33"/>
-      <c r="H76" s="33"/>
-      <c r="I76" s="33"/>
-      <c r="J76" s="33"/>
-      <c r="K76" s="33"/>
-    </row>
-    <row r="77" spans="2:11">
-      <c r="B77" s="34" t="s">
-        <v>30</v>
-      </c>
-      <c r="C77" s="34"/>
-      <c r="D77" s="34"/>
-      <c r="E77" s="34"/>
-      <c r="F77" s="34"/>
-      <c r="G77" s="34"/>
-      <c r="H77" s="34"/>
-      <c r="I77" s="34"/>
-      <c r="J77" s="34"/>
-      <c r="K77" s="34"/>
+      <c r="C77" s="31"/>
+      <c r="D77" s="31"/>
+      <c r="E77" s="31"/>
+      <c r="F77" s="31"/>
+      <c r="G77" s="31"/>
+      <c r="H77" s="31"/>
+      <c r="I77" s="31"/>
+      <c r="J77" s="31"/>
+      <c r="K77" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A3:L3"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="J34:K34"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="E70:F70"/>
+    <mergeCell ref="B75:K75"/>
+    <mergeCell ref="B76:K76"/>
+    <mergeCell ref="B77:K77"/>
     <mergeCell ref="B48:C48"/>
     <mergeCell ref="J48:K48"/>
     <mergeCell ref="B61:C61"/>
     <mergeCell ref="J61:K61"/>
     <mergeCell ref="I65:J65"/>
     <mergeCell ref="G65:H65"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="E70:F70"/>
-    <mergeCell ref="B75:K75"/>
-    <mergeCell ref="B76:K76"/>
-    <mergeCell ref="B77:K77"/>
+    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="J34:K34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.69791666666666696" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="55" fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -1910,17 +1832,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ed9e16c4-1eed-4354-9871-d189e3c9a5fe">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="98cd172a-97c0-47c0-9786-0a002598d91f" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000DB3645FD009914E90050545EEE2BF69" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a536e2a6beb9bff2427a440391878615">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ed9e16c4-1eed-4354-9871-d189e3c9a5fe" xmlns:ns3="98cd172a-97c0-47c0-9786-0a002598d91f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4eeb6a56791bed3cae1faef355ed4e3e" ns2:_="" ns3:_="">
     <xsd:import namespace="ed9e16c4-1eed-4354-9871-d189e3c9a5fe"/>
@@ -2175,6 +2086,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ed9e16c4-1eed-4354-9871-d189e3c9a5fe">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="98cd172a-97c0-47c0-9786-0a002598d91f" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F241F43E-FEE9-4AB6-ACF6-C186E160F71A}">
   <ds:schemaRefs>
@@ -2184,17 +2106,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6E9A4A9-1CDC-4B45-B233-F0B8036F5C80}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ed9e16c4-1eed-4354-9871-d189e3c9a5fe"/>
-    <ds:schemaRef ds:uri="98cd172a-97c0-47c0-9786-0a002598d91f"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E5ADF89-E94C-4A91-8192-FB55CE9EC04C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2211,4 +2122,15 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6E9A4A9-1CDC-4B45-B233-F0B8036F5C80}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ed9e16c4-1eed-4354-9871-d189e3c9a5fe"/>
+    <ds:schemaRef ds:uri="98cd172a-97c0-47c0-9786-0a002598d91f"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>